<commit_message>
Backup QR Scanner data - 2025-12-16T11:43:45.039Z - Cache Bust: 1765885425039
</commit_message>
<xml_diff>
--- a/log_history/Y4_B2526_Chest_scanner1765273993650_d6fe3b4260ce8e2ed0cf653b3c85db8e38decb904fade68bdc834d7dbd2e7ad3.xlsx
+++ b/log_history/Y4_B2526_Chest_scanner1765273993650_d6fe3b4260ce8e2ed0cf653b3c85db8e38decb904fade68bdc834d7dbd2e7ad3.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Chest" sheetId="1" r:id="rId1"/>
+    <sheet name="Scanner" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F69"/>
+  <dimension ref="A1:F74"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -424,19 +424,19 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>212119</v>
+        <v>200405</v>
       </c>
       <c r="B2" t="str">
         <v>Chest</v>
       </c>
       <c r="C2" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D2" t="str">
-        <v>11:53:52</v>
+        <v>13:32:38</v>
       </c>
       <c r="E2" t="str">
-        <v>Scan</v>
+        <v>Manual</v>
       </c>
       <c r="F2" t="str">
         <v>abdallahashraf2023@gmail.com</v>
@@ -444,19 +444,19 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>212291</v>
+        <v>200359</v>
       </c>
       <c r="B3" t="str">
         <v>Chest</v>
       </c>
       <c r="C3" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D3" t="str">
-        <v>11:54:00</v>
+        <v>13:32:43</v>
       </c>
       <c r="E3" t="str">
-        <v>Scan</v>
+        <v>Manual</v>
       </c>
       <c r="F3" t="str">
         <v>abdallahashraf2023@gmail.com</v>
@@ -464,19 +464,19 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>200344</v>
+        <v>200003</v>
       </c>
       <c r="B4" t="str">
         <v>Chest</v>
       </c>
       <c r="C4" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D4" t="str">
-        <v>11:54:18</v>
+        <v>13:32:48</v>
       </c>
       <c r="E4" t="str">
-        <v>Scan</v>
+        <v>Manual</v>
       </c>
       <c r="F4" t="str">
         <v>abdallahashraf2023@gmail.com</v>
@@ -484,19 +484,19 @@
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>212598</v>
+        <v>212477</v>
       </c>
       <c r="B5" t="str">
         <v>Chest</v>
       </c>
       <c r="C5" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D5" t="str">
-        <v>11:54:19</v>
+        <v>13:32:50</v>
       </c>
       <c r="E5" t="str">
-        <v>Manual</v>
+        <v>Scan</v>
       </c>
       <c r="F5" t="str">
         <v>abdallahashraf2023@gmail.com</v>
@@ -504,19 +504,19 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>200163</v>
+        <v>222064</v>
       </c>
       <c r="B6" t="str">
         <v>Chest</v>
       </c>
       <c r="C6" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D6" t="str">
-        <v>11:54:21</v>
+        <v>13:32:55</v>
       </c>
       <c r="E6" t="str">
-        <v>Scan</v>
+        <v>Manual</v>
       </c>
       <c r="F6" t="str">
         <v>abdallahashraf2023@gmail.com</v>
@@ -524,19 +524,19 @@
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>200116</v>
+        <v>222062</v>
       </c>
       <c r="B7" t="str">
         <v>Chest</v>
       </c>
       <c r="C7" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D7" t="str">
-        <v>11:54:28</v>
+        <v>13:33:04</v>
       </c>
       <c r="E7" t="str">
-        <v>Scan</v>
+        <v>Manual</v>
       </c>
       <c r="F7" t="str">
         <v>abdallahashraf2023@gmail.com</v>
@@ -544,16 +544,16 @@
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>212477</v>
+        <v>200228</v>
       </c>
       <c r="B8" t="str">
         <v>Chest</v>
       </c>
       <c r="C8" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D8" t="str">
-        <v>11:54:31</v>
+        <v>13:33:32</v>
       </c>
       <c r="E8" t="str">
         <v>Scan</v>
@@ -564,19 +564,19 @@
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>212455</v>
+        <v>200116</v>
       </c>
       <c r="B9" t="str">
         <v>Chest</v>
       </c>
       <c r="C9" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D9" t="str">
-        <v>11:54:40</v>
+        <v>13:33:34</v>
       </c>
       <c r="E9" t="str">
-        <v>Manual</v>
+        <v>Scan</v>
       </c>
       <c r="F9" t="str">
         <v>abdallahashraf2023@gmail.com</v>
@@ -584,16 +584,16 @@
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>212195</v>
+        <v>212373</v>
       </c>
       <c r="B10" t="str">
         <v>Chest</v>
       </c>
       <c r="C10" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D10" t="str">
-        <v>11:54:47</v>
+        <v>13:33:51</v>
       </c>
       <c r="E10" t="str">
         <v>Scan</v>
@@ -604,19 +604,19 @@
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>212283</v>
+        <v>212347</v>
       </c>
       <c r="B11" t="str">
         <v>Chest</v>
       </c>
       <c r="C11" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D11" t="str">
-        <v>11:54:53</v>
+        <v>13:33:54</v>
       </c>
       <c r="E11" t="str">
-        <v>Manual</v>
+        <v>Scan</v>
       </c>
       <c r="F11" t="str">
         <v>abdallahashraf2023@gmail.com</v>
@@ -624,19 +624,19 @@
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>212433</v>
+        <v>212155</v>
       </c>
       <c r="B12" t="str">
         <v>Chest</v>
       </c>
       <c r="C12" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D12" t="str">
-        <v>11:55:00</v>
+        <v>13:33:58</v>
       </c>
       <c r="E12" t="str">
-        <v>Manual</v>
+        <v>Scan</v>
       </c>
       <c r="F12" t="str">
         <v>abdallahashraf2023@gmail.com</v>
@@ -644,16 +644,16 @@
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>200490</v>
+        <v>200163</v>
       </c>
       <c r="B13" t="str">
         <v>Chest</v>
       </c>
       <c r="C13" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D13" t="str">
-        <v>11:55:04</v>
+        <v>13:34:00</v>
       </c>
       <c r="E13" t="str">
         <v>Scan</v>
@@ -664,16 +664,16 @@
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>200468</v>
+        <v>212254</v>
       </c>
       <c r="B14" t="str">
         <v>Chest</v>
       </c>
       <c r="C14" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D14" t="str">
-        <v>11:55:12</v>
+        <v>13:34:14</v>
       </c>
       <c r="E14" t="str">
         <v>Manual</v>
@@ -690,10 +690,10 @@
         <v>Chest</v>
       </c>
       <c r="C15" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D15" t="str">
-        <v>11:55:18</v>
+        <v>13:34:20</v>
       </c>
       <c r="E15" t="str">
         <v>Manual</v>
@@ -704,19 +704,19 @@
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>221761</v>
+        <v>212245</v>
       </c>
       <c r="B16" t="str">
         <v>Chest</v>
       </c>
       <c r="C16" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D16" t="str">
-        <v>11:55:19</v>
+        <v>13:34:39</v>
       </c>
       <c r="E16" t="str">
-        <v>Scan</v>
+        <v>Manual</v>
       </c>
       <c r="F16" t="str">
         <v>abdallahashraf2023@gmail.com</v>
@@ -724,16 +724,16 @@
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>210435</v>
+        <v>212154</v>
       </c>
       <c r="B17" t="str">
         <v>Chest</v>
       </c>
       <c r="C17" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D17" t="str">
-        <v>11:55:40</v>
+        <v>13:34:43</v>
       </c>
       <c r="E17" t="str">
         <v>Manual</v>
@@ -744,19 +744,19 @@
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>210301</v>
+        <v>221786</v>
       </c>
       <c r="B18" t="str">
         <v>Chest</v>
       </c>
       <c r="C18" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D18" t="str">
-        <v>11:55:42</v>
+        <v>13:34:57</v>
       </c>
       <c r="E18" t="str">
-        <v>Scan</v>
+        <v>Manual</v>
       </c>
       <c r="F18" t="str">
         <v>abdallahashraf2023@gmail.com</v>
@@ -764,19 +764,19 @@
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>212431</v>
+        <v>212193</v>
       </c>
       <c r="B19" t="str">
         <v>Chest</v>
       </c>
       <c r="C19" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D19" t="str">
-        <v>11:55:47</v>
+        <v>13:35:03</v>
       </c>
       <c r="E19" t="str">
-        <v>Scan</v>
+        <v>Manual</v>
       </c>
       <c r="F19" t="str">
         <v>abdallahashraf2023@gmail.com</v>
@@ -784,19 +784,19 @@
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>212347</v>
+        <v>212588</v>
       </c>
       <c r="B20" t="str">
         <v>Chest</v>
       </c>
       <c r="C20" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D20" t="str">
-        <v>11:55:49</v>
+        <v>13:35:20</v>
       </c>
       <c r="E20" t="str">
-        <v>Scan</v>
+        <v>Manual</v>
       </c>
       <c r="F20" t="str">
         <v>abdallahashraf2023@gmail.com</v>
@@ -804,16 +804,16 @@
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>212094</v>
+        <v>212307</v>
       </c>
       <c r="B21" t="str">
         <v>Chest</v>
       </c>
       <c r="C21" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D21" t="str">
-        <v>11:55:56</v>
+        <v>13:35:38</v>
       </c>
       <c r="E21" t="str">
         <v>Manual</v>
@@ -830,10 +830,10 @@
         <v>Chest</v>
       </c>
       <c r="C22" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D22" t="str">
-        <v>11:56:02</v>
+        <v>13:35:44</v>
       </c>
       <c r="E22" t="str">
         <v>Manual</v>
@@ -844,16 +844,16 @@
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>212258</v>
+        <v>222080</v>
       </c>
       <c r="B23" t="str">
         <v>Chest</v>
       </c>
       <c r="C23" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D23" t="str">
-        <v>11:56:07</v>
+        <v>13:35:48</v>
       </c>
       <c r="E23" t="str">
         <v>Manual</v>
@@ -864,16 +864,16 @@
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>212368</v>
+        <v>222078</v>
       </c>
       <c r="B24" t="str">
         <v>Chest</v>
       </c>
       <c r="C24" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D24" t="str">
-        <v>11:56:16</v>
+        <v>13:35:54</v>
       </c>
       <c r="E24" t="str">
         <v>Manual</v>
@@ -884,16 +884,16 @@
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>212135</v>
+        <v>212368</v>
       </c>
       <c r="B25" t="str">
         <v>Chest</v>
       </c>
       <c r="C25" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D25" t="str">
-        <v>11:56:22</v>
+        <v>13:35:59</v>
       </c>
       <c r="E25" t="str">
         <v>Manual</v>
@@ -904,16 +904,16 @@
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>212511</v>
+        <v>212320</v>
       </c>
       <c r="B26" t="str">
         <v>Chest</v>
       </c>
       <c r="C26" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D26" t="str">
-        <v>11:56:27</v>
+        <v>13:36:12</v>
       </c>
       <c r="E26" t="str">
         <v>Manual</v>
@@ -924,16 +924,16 @@
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>212123</v>
+        <v>212137</v>
       </c>
       <c r="B27" t="str">
         <v>Chest</v>
       </c>
       <c r="C27" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D27" t="str">
-        <v>11:56:32</v>
+        <v>13:36:19</v>
       </c>
       <c r="E27" t="str">
         <v>Manual</v>
@@ -944,16 +944,16 @@
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>212154</v>
+        <v>212195</v>
       </c>
       <c r="B28" t="str">
         <v>Chest</v>
       </c>
       <c r="C28" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D28" t="str">
-        <v>11:56:34</v>
+        <v>13:36:23</v>
       </c>
       <c r="E28" t="str">
         <v>Scan</v>
@@ -964,19 +964,19 @@
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>221786</v>
+        <v>212345</v>
       </c>
       <c r="B29" t="str">
         <v>Chest</v>
       </c>
       <c r="C29" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D29" t="str">
-        <v>11:56:41</v>
+        <v>13:36:28</v>
       </c>
       <c r="E29" t="str">
-        <v>Manual</v>
+        <v>Scan</v>
       </c>
       <c r="F29" t="str">
         <v>abdallahashraf2023@gmail.com</v>
@@ -984,19 +984,19 @@
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>221773</v>
+        <v>212346</v>
       </c>
       <c r="B30" t="str">
         <v>Chest</v>
       </c>
       <c r="C30" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D30" t="str">
-        <v>11:56:47</v>
+        <v>13:36:29</v>
       </c>
       <c r="E30" t="str">
-        <v>Manual</v>
+        <v>Scan</v>
       </c>
       <c r="F30" t="str">
         <v>abdallahashraf2023@gmail.com</v>
@@ -1004,19 +1004,19 @@
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>212248</v>
+        <v>212101</v>
       </c>
       <c r="B31" t="str">
         <v>Chest</v>
       </c>
       <c r="C31" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D31" t="str">
-        <v>11:56:53</v>
+        <v>13:36:33</v>
       </c>
       <c r="E31" t="str">
-        <v>Manual</v>
+        <v>Scan</v>
       </c>
       <c r="F31" t="str">
         <v>abdallahashraf2023@gmail.com</v>
@@ -1024,16 +1024,16 @@
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>212144</v>
+        <v>212094</v>
       </c>
       <c r="B32" t="str">
         <v>Chest</v>
       </c>
       <c r="C32" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D32" t="str">
-        <v>11:56:59</v>
+        <v>13:36:39</v>
       </c>
       <c r="E32" t="str">
         <v>Manual</v>
@@ -1044,19 +1044,19 @@
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>200228</v>
+        <v>212161</v>
       </c>
       <c r="B33" t="str">
         <v>Chest</v>
       </c>
       <c r="C33" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D33" t="str">
-        <v>11:57:04</v>
+        <v>13:36:45</v>
       </c>
       <c r="E33" t="str">
-        <v>Scan</v>
+        <v>Manual</v>
       </c>
       <c r="F33" t="str">
         <v>abdallahashraf2023@gmail.com</v>
@@ -1064,16 +1064,16 @@
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>212279</v>
+        <v>212333</v>
       </c>
       <c r="B34" t="str">
         <v>Chest</v>
       </c>
       <c r="C34" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D34" t="str">
-        <v>11:57:11</v>
+        <v>13:36:50</v>
       </c>
       <c r="E34" t="str">
         <v>Manual</v>
@@ -1084,19 +1084,19 @@
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>212320</v>
+        <v>212183</v>
       </c>
       <c r="B35" t="str">
         <v>Chest</v>
       </c>
       <c r="C35" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D35" t="str">
-        <v>11:57:13</v>
+        <v>13:36:57</v>
       </c>
       <c r="E35" t="str">
-        <v>Scan</v>
+        <v>Manual</v>
       </c>
       <c r="F35" t="str">
         <v>abdallahashraf2023@gmail.com</v>
@@ -1104,16 +1104,16 @@
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>212588</v>
+        <v>221689</v>
       </c>
       <c r="B36" t="str">
         <v>Chest</v>
       </c>
       <c r="C36" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D36" t="str">
-        <v>11:57:22</v>
+        <v>13:37:05</v>
       </c>
       <c r="E36" t="str">
         <v>Manual</v>
@@ -1124,19 +1124,19 @@
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>212362</v>
+        <v>212592</v>
       </c>
       <c r="B37" t="str">
         <v>Chest</v>
       </c>
       <c r="C37" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D37" t="str">
-        <v>11:57:24</v>
+        <v>13:37:19</v>
       </c>
       <c r="E37" t="str">
-        <v>Scan</v>
+        <v>Manual</v>
       </c>
       <c r="F37" t="str">
         <v>abdallahashraf2023@gmail.com</v>
@@ -1144,16 +1144,16 @@
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>212453</v>
+        <v>212258</v>
       </c>
       <c r="B38" t="str">
         <v>Chest</v>
       </c>
       <c r="C38" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D38" t="str">
-        <v>11:57:34</v>
+        <v>13:37:33</v>
       </c>
       <c r="E38" t="str">
         <v>Manual</v>
@@ -1164,19 +1164,19 @@
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>212254</v>
+        <v>212587</v>
       </c>
       <c r="B39" t="str">
         <v>Chest</v>
       </c>
       <c r="C39" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D39" t="str">
-        <v>11:57:40</v>
+        <v>13:37:38</v>
       </c>
       <c r="E39" t="str">
-        <v>Manual</v>
+        <v>Scan</v>
       </c>
       <c r="F39" t="str">
         <v>abdallahashraf2023@gmail.com</v>
@@ -1184,19 +1184,19 @@
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>212324</v>
+        <v>212445</v>
       </c>
       <c r="B40" t="str">
         <v>Chest</v>
       </c>
       <c r="C40" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D40" t="str">
-        <v>11:57:46</v>
+        <v>13:37:41</v>
       </c>
       <c r="E40" t="str">
-        <v>Manual</v>
+        <v>Scan</v>
       </c>
       <c r="F40" t="str">
         <v>abdallahashraf2023@gmail.com</v>
@@ -1204,19 +1204,19 @@
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>212205</v>
+        <v>200344</v>
       </c>
       <c r="B41" t="str">
         <v>Chest</v>
       </c>
       <c r="C41" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D41" t="str">
-        <v>11:57:52</v>
+        <v>13:37:44</v>
       </c>
       <c r="E41" t="str">
-        <v>Manual</v>
+        <v>Scan</v>
       </c>
       <c r="F41" t="str">
         <v>abdallahashraf2023@gmail.com</v>
@@ -1224,16 +1224,16 @@
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>212346</v>
+        <v>212414</v>
       </c>
       <c r="B42" t="str">
         <v>Chest</v>
       </c>
       <c r="C42" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D42" t="str">
-        <v>11:57:54</v>
+        <v>13:37:48</v>
       </c>
       <c r="E42" t="str">
         <v>Scan</v>
@@ -1244,16 +1244,16 @@
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>212440</v>
+        <v>212511</v>
       </c>
       <c r="B43" t="str">
         <v>Chest</v>
       </c>
       <c r="C43" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D43" t="str">
-        <v>11:58:30</v>
+        <v>13:37:55</v>
       </c>
       <c r="E43" t="str">
         <v>Manual</v>
@@ -1264,19 +1264,19 @@
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>212414</v>
+        <v>212440</v>
       </c>
       <c r="B44" t="str">
         <v>Chest</v>
       </c>
       <c r="C44" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D44" t="str">
-        <v>11:58:33</v>
+        <v>13:38:04</v>
       </c>
       <c r="E44" t="str">
-        <v>Scan</v>
+        <v>Manual</v>
       </c>
       <c r="F44" t="str">
         <v>abdallahashraf2023@gmail.com</v>
@@ -1284,16 +1284,16 @@
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>212479</v>
+        <v>212362</v>
       </c>
       <c r="B45" t="str">
         <v>Chest</v>
       </c>
       <c r="C45" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D45" t="str">
-        <v>11:58:43</v>
+        <v>13:38:08</v>
       </c>
       <c r="E45" t="str">
         <v>Manual</v>
@@ -1304,16 +1304,16 @@
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>212377</v>
+        <v>200490</v>
       </c>
       <c r="B46" t="str">
         <v>Chest</v>
       </c>
       <c r="C46" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D46" t="str">
-        <v>11:58:54</v>
+        <v>13:38:11</v>
       </c>
       <c r="E46" t="str">
         <v>Scan</v>
@@ -1324,19 +1324,19 @@
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>212266</v>
+        <v>210301</v>
       </c>
       <c r="B47" t="str">
         <v>Chest</v>
       </c>
       <c r="C47" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D47" t="str">
-        <v>11:58:57</v>
+        <v>13:38:12</v>
       </c>
       <c r="E47" t="str">
-        <v>Manual</v>
+        <v>Scan</v>
       </c>
       <c r="F47" t="str">
         <v>abdallahashraf2023@gmail.com</v>
@@ -1344,16 +1344,16 @@
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>212101</v>
+        <v>212324</v>
       </c>
       <c r="B48" t="str">
         <v>Chest</v>
       </c>
       <c r="C48" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D48" t="str">
-        <v>11:59:03</v>
+        <v>13:38:14</v>
       </c>
       <c r="E48" t="str">
         <v>Scan</v>
@@ -1364,16 +1364,16 @@
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>212587</v>
+        <v>212205</v>
       </c>
       <c r="B49" t="str">
         <v>Chest</v>
       </c>
       <c r="C49" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D49" t="str">
-        <v>11:59:10</v>
+        <v>13:38:20</v>
       </c>
       <c r="E49" t="str">
         <v>Manual</v>
@@ -1384,16 +1384,16 @@
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>212245</v>
+        <v>210435</v>
       </c>
       <c r="B50" t="str">
         <v>Chest</v>
       </c>
       <c r="C50" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D50" t="str">
-        <v>11:59:16</v>
+        <v>13:38:27</v>
       </c>
       <c r="E50" t="str">
         <v>Manual</v>
@@ -1404,19 +1404,19 @@
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>212373</v>
+        <v>212279</v>
       </c>
       <c r="B51" t="str">
         <v>Chest</v>
       </c>
       <c r="C51" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D51" t="str">
-        <v>11:59:18</v>
+        <v>13:38:32</v>
       </c>
       <c r="E51" t="str">
-        <v>Scan</v>
+        <v>Manual</v>
       </c>
       <c r="F51" t="str">
         <v>abdallahashraf2023@gmail.com</v>
@@ -1424,16 +1424,16 @@
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>222064</v>
+        <v>212266</v>
       </c>
       <c r="B52" t="str">
         <v>Chest</v>
       </c>
       <c r="C52" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D52" t="str">
-        <v>11:59:32</v>
+        <v>13:38:38</v>
       </c>
       <c r="E52" t="str">
         <v>Manual</v>
@@ -1444,19 +1444,19 @@
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>212193</v>
+        <v>212598</v>
       </c>
       <c r="B53" t="str">
         <v>Chest</v>
       </c>
       <c r="C53" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D53" t="str">
-        <v>11:59:37</v>
+        <v>13:38:43</v>
       </c>
       <c r="E53" t="str">
-        <v>Scan</v>
+        <v>Manual</v>
       </c>
       <c r="F53" t="str">
         <v>abdallahashraf2023@gmail.com</v>
@@ -1464,19 +1464,19 @@
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>212345</v>
+        <v>212479</v>
       </c>
       <c r="B54" t="str">
         <v>Chest</v>
       </c>
       <c r="C54" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D54" t="str">
-        <v>11:59:43</v>
+        <v>13:38:50</v>
       </c>
       <c r="E54" t="str">
-        <v>Scan</v>
+        <v>Manual</v>
       </c>
       <c r="F54" t="str">
         <v>abdallahashraf2023@gmail.com</v>
@@ -1484,16 +1484,16 @@
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>212155</v>
+        <v>212084</v>
       </c>
       <c r="B55" t="str">
         <v>Chest</v>
       </c>
       <c r="C55" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D55" t="str">
-        <v>11:59:49</v>
+        <v>13:39:01</v>
       </c>
       <c r="E55" t="str">
         <v>Manual</v>
@@ -1504,16 +1504,16 @@
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>200405</v>
+        <v>212135</v>
       </c>
       <c r="B56" t="str">
         <v>Chest</v>
       </c>
       <c r="C56" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D56" t="str">
-        <v>12:00:36</v>
+        <v>13:39:07</v>
       </c>
       <c r="E56" t="str">
         <v>Manual</v>
@@ -1524,19 +1524,19 @@
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v>200359</v>
+        <v>212377</v>
       </c>
       <c r="B57" t="str">
         <v>Chest</v>
       </c>
       <c r="C57" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D57" t="str">
-        <v>12:00:48</v>
+        <v>13:39:09</v>
       </c>
       <c r="E57" t="str">
-        <v>Manual</v>
+        <v>Scan</v>
       </c>
       <c r="F57" t="str">
         <v>abdallahashraf2023@gmail.com</v>
@@ -1544,16 +1544,16 @@
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>222102</v>
+        <v>212123</v>
       </c>
       <c r="B58" t="str">
         <v>Chest</v>
       </c>
       <c r="C58" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D58" t="str">
-        <v>12:00:56</v>
+        <v>13:39:14</v>
       </c>
       <c r="E58" t="str">
         <v>Manual</v>
@@ -1564,19 +1564,19 @@
     </row>
     <row r="59">
       <c r="A59" t="str">
-        <v>221891</v>
+        <v>212119</v>
       </c>
       <c r="B59" t="str">
         <v>Chest</v>
       </c>
       <c r="C59" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D59" t="str">
-        <v>12:01:10</v>
+        <v>13:39:17</v>
       </c>
       <c r="E59" t="str">
-        <v>Manual</v>
+        <v>Scan</v>
       </c>
       <c r="F59" t="str">
         <v>abdallahashraf2023@gmail.com</v>
@@ -1584,16 +1584,16 @@
     </row>
     <row r="60">
       <c r="A60" t="str">
-        <v>200423</v>
+        <v>212455</v>
       </c>
       <c r="B60" t="str">
         <v>Chest</v>
       </c>
       <c r="C60" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D60" t="str">
-        <v>12:01:17</v>
+        <v>13:39:25</v>
       </c>
       <c r="E60" t="str">
         <v>Manual</v>
@@ -1604,16 +1604,16 @@
     </row>
     <row r="61">
       <c r="A61" t="str">
-        <v>212121</v>
+        <v>212315</v>
       </c>
       <c r="B61" t="str">
         <v>Chest</v>
       </c>
       <c r="C61" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D61" t="str">
-        <v>12:01:26</v>
+        <v>13:39:27</v>
       </c>
       <c r="E61" t="str">
         <v>Scan</v>
@@ -1624,19 +1624,19 @@
     </row>
     <row r="62">
       <c r="A62" t="str">
-        <v>212333</v>
+        <v>212314</v>
       </c>
       <c r="B62" t="str">
         <v>Chest</v>
       </c>
       <c r="C62" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D62" t="str">
-        <v>12:01:37</v>
+        <v>13:39:30</v>
       </c>
       <c r="E62" t="str">
-        <v>Manual</v>
+        <v>Scan</v>
       </c>
       <c r="F62" t="str">
         <v>abdallahashraf2023@gmail.com</v>
@@ -1644,16 +1644,16 @@
     </row>
     <row r="63">
       <c r="A63" t="str">
-        <v>212306</v>
+        <v>212291</v>
       </c>
       <c r="B63" t="str">
         <v>Chest</v>
       </c>
       <c r="C63" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D63" t="str">
-        <v>12:01:42</v>
+        <v>13:39:40</v>
       </c>
       <c r="E63" t="str">
         <v>Manual</v>
@@ -1664,16 +1664,16 @@
     </row>
     <row r="64">
       <c r="A64" t="str">
-        <v>212161</v>
+        <v>212453</v>
       </c>
       <c r="B64" t="str">
         <v>Chest</v>
       </c>
       <c r="C64" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D64" t="str">
-        <v>12:01:48</v>
+        <v>13:39:46</v>
       </c>
       <c r="E64" t="str">
         <v>Manual</v>
@@ -1684,16 +1684,16 @@
     </row>
     <row r="65">
       <c r="A65" t="str">
-        <v>212592</v>
+        <v>212144</v>
       </c>
       <c r="B65" t="str">
         <v>Chest</v>
       </c>
       <c r="C65" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D65" t="str">
-        <v>12:01:56</v>
+        <v>13:39:52</v>
       </c>
       <c r="E65" t="str">
         <v>Manual</v>
@@ -1704,16 +1704,16 @@
     </row>
     <row r="66">
       <c r="A66" t="str">
-        <v>212445</v>
+        <v>212431</v>
       </c>
       <c r="B66" t="str">
         <v>Chest</v>
       </c>
       <c r="C66" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D66" t="str">
-        <v>12:02:05</v>
+        <v>13:39:54</v>
       </c>
       <c r="E66" t="str">
         <v>Scan</v>
@@ -1724,16 +1724,16 @@
     </row>
     <row r="67">
       <c r="A67" t="str">
-        <v>212183</v>
+        <v>212283</v>
       </c>
       <c r="B67" t="str">
         <v>Chest</v>
       </c>
       <c r="C67" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D67" t="str">
-        <v>12:02:07</v>
+        <v>13:40:00</v>
       </c>
       <c r="E67" t="str">
         <v>Manual</v>
@@ -1744,16 +1744,16 @@
     </row>
     <row r="68">
       <c r="A68" t="str">
-        <v>212137</v>
+        <v>212306</v>
       </c>
       <c r="B68" t="str">
         <v>Chest</v>
       </c>
       <c r="C68" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D68" t="str">
-        <v>12:02:18</v>
+        <v>13:40:37</v>
       </c>
       <c r="E68" t="str">
         <v>Manual</v>
@@ -1764,27 +1764,127 @@
     </row>
     <row r="69">
       <c r="A69" t="str">
-        <v>200003</v>
+        <v>210937</v>
       </c>
       <c r="B69" t="str">
         <v>Chest</v>
       </c>
       <c r="C69" t="str">
-        <v>09/12/2025</v>
+        <v>16/12/2025</v>
       </c>
       <c r="D69" t="str">
-        <v>12:02:24</v>
+        <v>13:40:44</v>
       </c>
       <c r="E69" t="str">
         <v>Manual</v>
       </c>
       <c r="F69" t="str">
+        <v>abdallahashraf2023@gmail.com</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="str">
+        <v>212121</v>
+      </c>
+      <c r="B70" t="str">
+        <v>Chest</v>
+      </c>
+      <c r="C70" t="str">
+        <v>16/12/2025</v>
+      </c>
+      <c r="D70" t="str">
+        <v>13:40:48</v>
+      </c>
+      <c r="E70" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F70" t="str">
+        <v>abdallahashraf2023@gmail.com</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="str">
+        <v>221885</v>
+      </c>
+      <c r="B71" t="str">
+        <v>Chest</v>
+      </c>
+      <c r="C71" t="str">
+        <v>16/12/2025</v>
+      </c>
+      <c r="D71" t="str">
+        <v>13:40:51</v>
+      </c>
+      <c r="E71" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F71" t="str">
+        <v>abdallahashraf2023@gmail.com</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="str">
+        <v>221773</v>
+      </c>
+      <c r="B72" t="str">
+        <v>Chest</v>
+      </c>
+      <c r="C72" t="str">
+        <v>16/12/2025</v>
+      </c>
+      <c r="D72" t="str">
+        <v>13:41:07</v>
+      </c>
+      <c r="E72" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F72" t="str">
+        <v>abdallahashraf2023@gmail.com</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="str">
+        <v>222102</v>
+      </c>
+      <c r="B73" t="str">
+        <v>Chest</v>
+      </c>
+      <c r="C73" t="str">
+        <v>16/12/2025</v>
+      </c>
+      <c r="D73" t="str">
+        <v>13:41:12</v>
+      </c>
+      <c r="E73" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F73" t="str">
+        <v>abdallahashraf2023@gmail.com</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="str">
+        <v>221891</v>
+      </c>
+      <c r="B74" t="str">
+        <v>Chest</v>
+      </c>
+      <c r="C74" t="str">
+        <v>16/12/2025</v>
+      </c>
+      <c r="D74" t="str">
+        <v>13:41:21</v>
+      </c>
+      <c r="E74" t="str">
+        <v>Manual</v>
+      </c>
+      <c r="F74" t="str">
         <v>abdallahashraf2023@gmail.com</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F69"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F74"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>